<commit_message>
Fix Tea Inventory survey
</commit_message>
<xml_diff>
--- a/app/config/tables/Tea_inventory/forms/Tea_inventory/Tea_inventory.xlsx
+++ b/app/config/tables/Tea_inventory/forms/Tea_inventory/Tea_inventory.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27224"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maegan/Documents/app-designer/app/config/tables/Tea_inventory/forms/Tea_inventory/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4380" yWindow="1860" windowWidth="33020" windowHeight="21800" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="4380" yWindow="1860" windowWidth="33020" windowHeight="21800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -15,6 +20,9 @@
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -199,9 +207,6 @@
     <t>select_one</t>
   </si>
   <si>
-    <t>Choose the tea type ID number.</t>
-  </si>
-  <si>
     <t>[ '0' ]</t>
   </si>
   <si>
@@ -260,6 +265,9 @@
   </si>
   <si>
     <t>config/tables/Tea_inventory/html/Tea_inventory_list.html</t>
+  </si>
+  <si>
+    <t>Choose the tea type.</t>
   </si>
 </sst>
 </file>
@@ -372,6 +380,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -699,18 +712,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="21.83203125" customWidth="1"/>
     <col min="5" max="5" width="34.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="30">
+    <row r="1" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -766,7 +779,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
         <v>21</v>
       </c>
@@ -780,7 +793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
         <v>57</v>
       </c>
@@ -791,18 +804,18 @@
         <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="J3" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>57</v>
       </c>
       <c r="D4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E4" t="s">
         <v>22</v>
@@ -814,12 +827,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
         <v>57</v>
       </c>
       <c r="D5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E5" t="s">
         <v>23</v>
@@ -831,12 +844,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
         <v>57</v>
       </c>
       <c r="D6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E6" t="s">
         <v>24</v>
@@ -848,12 +861,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
         <v>57</v>
       </c>
       <c r="D7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E7" t="s">
         <v>25</v>
@@ -865,9 +878,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E8" t="s">
         <v>26</v>
@@ -879,46 +892,46 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E9" t="s">
         <v>27</v>
       </c>
       <c r="F9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J9" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E10" t="s">
         <v>28</v>
       </c>
       <c r="F10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J10" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
         <v>57</v>
       </c>
       <c r="D11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E11" t="s">
+        <v>72</v>
+      </c>
+      <c r="F11" t="s">
         <v>73</v>
-      </c>
-      <c r="F11" t="s">
-        <v>74</v>
       </c>
       <c r="J11" t="b">
         <v>1</v>
@@ -927,11 +940,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -943,9 +951,9 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -956,7 +964,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -964,7 +972,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -972,7 +980,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -982,11 +990,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -998,7 +1001,7 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
     <col min="2" max="2" width="21.5" customWidth="1"/>
@@ -1009,7 +1012,7 @@
     <col min="7" max="7" width="32.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>47</v>
       </c>
@@ -1032,7 +1035,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -1046,46 +1049,41 @@
         <v>56</v>
       </c>
       <c r="E2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="F2" t="s">
-        <v>59</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
         <v>55</v>
       </c>
       <c r="C3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>71</v>
-      </c>
-      <c r="F3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1093,24 +1091,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1119,7 +1117,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -1136,7 +1134,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -1150,10 +1148,10 @@
         <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -1167,17 +1165,12 @@
         <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1189,50 +1182,45 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>65</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>66</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" t="s">
         <v>67</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" t="s">
         <v>68</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C3" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>